<commit_message>
disable send back tickets flow
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Venkatesh_Singamsitt\Desktop\Bombardier-100\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA7F086C-964B-415E-A1F0-CCB6DB2531D5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D313E19-1E73-47D2-A920-F70ECB412D00}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="23280" windowHeight="12600" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="23280" windowHeight="12750" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5604" uniqueCount="2301">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5608" uniqueCount="2305">
   <si>
     <t>Name</t>
   </si>
@@ -6936,13 +6936,25 @@
   </si>
   <si>
     <t>Bombardier-100 TechnicalExcepEmail</t>
+  </si>
+  <si>
+    <t>BotQueueUrl</t>
+  </si>
+  <si>
+    <t>Bombardier-100 Botqueue Url</t>
+  </si>
+  <si>
+    <t>Bombardier-100 Worknotes Reroute</t>
+  </si>
+  <si>
+    <t>RerouteWorknotes</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -6970,6 +6982,12 @@
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF4E5E65"/>
+      <name val="Arial"/>
       <family val="2"/>
     </font>
     <font>
@@ -7040,7 +7058,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -7075,6 +7093,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -9677,10 +9696,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -9762,8 +9782,22 @@
         <v>2298</v>
       </c>
     </row>
-    <row r="7" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="8" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="7" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>2301</v>
+      </c>
+      <c r="B7" s="16" t="s">
+        <v>2302</v>
+      </c>
+    </row>
+    <row r="8" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>2304</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>2303</v>
+      </c>
+    </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="10" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="11" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -10766,8 +10800,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19C42DCF-8AB3-41A7-B381-1E23322A149C}">
   <dimension ref="A1:J606"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -16083,7 +16117,7 @@
         <v>63</v>
       </c>
       <c r="G183" t="s">
-        <v>241</v>
+        <v>1215</v>
       </c>
       <c r="H183" s="8" t="s">
         <v>242</v>
@@ -16112,7 +16146,7 @@
         <v>63</v>
       </c>
       <c r="G184" t="s">
-        <v>241</v>
+        <v>1215</v>
       </c>
       <c r="H184" s="8" t="s">
         <v>242</v>
@@ -16953,7 +16987,7 @@
         <v>63</v>
       </c>
       <c r="G213" t="s">
-        <v>241</v>
+        <v>1215</v>
       </c>
       <c r="H213" s="8" t="s">
         <v>242</v>
@@ -20871,7 +20905,7 @@
         <v>63</v>
       </c>
       <c r="G348" t="s">
-        <v>241</v>
+        <v>1215</v>
       </c>
       <c r="H348" s="8" t="s">
         <v>242</v>
@@ -28621,6 +28655,7 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:J606" xr:uid="{CEC1A23C-044E-442B-9D30-837C1AD0F179}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>